<commit_message>
Actualizado todo el proyecto | Suprimidos Archivos temporales y resultados
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -3315,8 +3315,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40311,8 +40311,8 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40472,7 +40472,7 @@
         <v>163</v>
       </c>
       <c r="B16" s="168">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C16" s="169" t="s">
         <v>164</v>
@@ -40884,18 +40884,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Fecha xmlns="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a696cb9f-a21f-4396-ad55-16500bd1db7d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000C3846A8090354C9F592304855C6AE6" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf99c70284dc6984c97de95d99e140cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94" xmlns:ns3="a696cb9f-a21f-4396-ad55-16500bd1db7d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="29fb5f7eced63397a5e4c4278e51959c" ns2:_="" ns3:_="">
     <xsd:import namespace="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94"/>
@@ -41090,7 +41078,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -41099,18 +41087,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5D3924B-CC86-4613-BD6C-1F0D9761680A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94"/>
-    <ds:schemaRef ds:uri="a696cb9f-a21f-4396-ad55-16500bd1db7d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Fecha xmlns="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a696cb9f-a21f-4396-ad55-16500bd1db7d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{872F172B-9105-4BB3-9F57-86A1C7BE3A9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41129,10 +41118,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E41B7D-B428-4B54-A5CB-31F7E4F8365B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5D3924B-CC86-4613-BD6C-1F0D9761680A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9a0a112e-dafe-4d0c-9f22-58c1f2fd1b94"/>
+    <ds:schemaRef ds:uri="a696cb9f-a21f-4396-ad55-16500bd1db7d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>